<commit_message>
fix(gui) step 1 and 2
</commit_message>
<xml_diff>
--- a/server/LISTAS/ma/ARANDELA CHAPISTA y comunes.xlsx
+++ b/server/LISTAS/ma/ARANDELA CHAPISTA y comunes.xlsx
@@ -904,7 +904,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="19" t="n">
-        <v>45308</v>
+        <v>45309</v>
       </c>
       <c r="F1" s="40" t="n"/>
       <c r="G1" s="40" t="n"/>
@@ -988,7 +988,7 @@
       </c>
       <c r="C33" s="44" t="n"/>
       <c r="D33" s="9" t="n">
-        <v>3287.585</v>
+        <v>5030.479</v>
       </c>
     </row>
     <row r="34" ht="16.5" customHeight="1" s="42">
@@ -1002,7 +1002,7 @@
       </c>
       <c r="C34" s="44" t="n"/>
       <c r="D34" s="9" t="n">
-        <v>2470.096</v>
+        <v>3779.603</v>
       </c>
     </row>
     <row r="35" ht="16.5" customHeight="1" s="42">
@@ -1016,7 +1016,7 @@
       </c>
       <c r="C35" s="44" t="n"/>
       <c r="D35" s="9" t="n">
-        <v>2131.561</v>
+        <v>3261.594</v>
       </c>
     </row>
     <row r="36" ht="16.5" customHeight="1" s="42">
@@ -1030,7 +1030,7 @@
       </c>
       <c r="C36" s="44" t="n"/>
       <c r="D36" s="9" t="n">
-        <v>1914.227</v>
+        <v>2929.043</v>
       </c>
     </row>
     <row r="37" ht="16.5" customHeight="1" s="42">
@@ -1044,7 +1044,7 @@
       </c>
       <c r="C37" s="44" t="n"/>
       <c r="D37" s="9" t="n">
-        <v>1914.227</v>
+        <v>2929.043</v>
       </c>
     </row>
     <row r="38" ht="16.5" customHeight="1" s="42">
@@ -1058,7 +1058,7 @@
       </c>
       <c r="C38" s="44" t="n"/>
       <c r="D38" s="9" t="n">
-        <v>1614.548</v>
+        <v>2470.491</v>
       </c>
     </row>
     <row r="39" ht="16.5" customHeight="1" s="42">
@@ -1072,7 +1072,7 @@
       </c>
       <c r="C39" s="44" t="n"/>
       <c r="D39" s="9" t="n">
-        <v>1614.548</v>
+        <v>2470.491</v>
       </c>
     </row>
     <row r="40" ht="16.5" customHeight="1" s="42">
@@ -1086,7 +1086,7 @@
       </c>
       <c r="C40" s="44" t="n"/>
       <c r="D40" s="9" t="n">
-        <v>1614.548</v>
+        <v>2470.491</v>
       </c>
     </row>
     <row r="41" ht="16.5" customHeight="1" s="42">
@@ -1100,7 +1100,7 @@
       </c>
       <c r="C41" s="44" t="n"/>
       <c r="D41" s="9" t="n">
-        <v>1614.548</v>
+        <v>2470.491</v>
       </c>
     </row>
     <row r="42" ht="16.5" customHeight="1" s="42">
@@ -1114,7 +1114,7 @@
       </c>
       <c r="C42" s="44" t="n"/>
       <c r="D42" s="9" t="n">
-        <v>1614.548</v>
+        <v>2470.491</v>
       </c>
     </row>
     <row r="43" ht="16.5" customHeight="1" s="42">
@@ -1128,7 +1128,7 @@
       </c>
       <c r="C43" s="44" t="n"/>
       <c r="D43" s="9" t="n">
-        <v>1614.548</v>
+        <v>2470.491</v>
       </c>
     </row>
     <row r="44" ht="16.5" customHeight="1" s="42">
@@ -1144,7 +1144,7 @@
       </c>
       <c r="C44" s="44" t="n"/>
       <c r="D44" s="9" t="n">
-        <v>1614.548</v>
+        <v>2470.491</v>
       </c>
     </row>
     <row r="45" ht="16.5" customHeight="1" s="42">
@@ -1160,7 +1160,7 @@
       </c>
       <c r="C45" s="44" t="n"/>
       <c r="D45" s="9" t="n">
-        <v>1926.763</v>
+        <v>2948.224</v>
       </c>
     </row>
     <row r="46" ht="16.5" customHeight="1" s="42">
@@ -1176,7 +1176,7 @@
       </c>
       <c r="C46" s="44" t="n"/>
       <c r="D46" s="9" t="n">
-        <v>1926.763</v>
+        <v>2948.224</v>
       </c>
     </row>
     <row r="47" ht="16.5" customHeight="1" s="42">
@@ -1192,7 +1192,7 @@
       </c>
       <c r="C47" s="44" t="n"/>
       <c r="D47" s="9" t="n">
-        <v>1926.763</v>
+        <v>2948.224</v>
       </c>
     </row>
     <row r="49" ht="18" customHeight="1" s="42">
@@ -1234,7 +1234,7 @@
       </c>
       <c r="C51" s="44" t="n"/>
       <c r="D51" s="9" t="n">
-        <v>2808.644</v>
+        <v>4297.629</v>
       </c>
     </row>
     <row r="52" ht="18" customHeight="1" s="42">
@@ -1248,7 +1248,7 @@
       </c>
       <c r="C52" s="44" t="n"/>
       <c r="D52" s="9" t="n">
-        <v>2553.696</v>
+        <v>3907.523</v>
       </c>
     </row>
     <row r="53" ht="23.25" customHeight="1" s="42">
@@ -1262,7 +1262,7 @@
       </c>
       <c r="C53" s="44" t="n"/>
       <c r="D53" s="9" t="n">
-        <v>2131.561</v>
+        <v>3261.594</v>
       </c>
       <c r="E53" s="10" t="n"/>
       <c r="F53" s="10" t="n"/>
@@ -1280,7 +1280,7 @@
       </c>
       <c r="C54" s="44" t="n"/>
       <c r="D54" s="9" t="n">
-        <v>2131.561</v>
+        <v>3261.594</v>
       </c>
       <c r="E54" s="11" t="n"/>
       <c r="F54" s="11" t="n"/>
@@ -1350,37 +1350,37 @@
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D73:E73"/>
+    <mergeCell ref="B46:C46"/>
     <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="D77:E77"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B34:C34"/>
     <mergeCell ref="A11:E11"/>
-    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="A49:D49"/>
+    <mergeCell ref="B52:C52"/>
     <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="D77:E77"/>
-    <mergeCell ref="A31:D31"/>
-    <mergeCell ref="D76:E76"/>
     <mergeCell ref="B42:C42"/>
-    <mergeCell ref="A49:D49"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D74:E74"/>
     <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B34:C34"/>
     <mergeCell ref="B37:C37"/>
     <mergeCell ref="B40:C40"/>
-    <mergeCell ref="D74:E74"/>
-    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="B36:C36"/>
     <mergeCell ref="B51:C51"/>
-    <mergeCell ref="D73:E73"/>
-    <mergeCell ref="A10:H10"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B35:C35"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
   <pageSetup orientation="portrait" paperSize="9" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
refactor code and structure files
</commit_message>
<xml_diff>
--- a/server/LISTAS/ma/ARANDELA CHAPISTA y comunes.xlsx
+++ b/server/LISTAS/ma/ARANDELA CHAPISTA y comunes.xlsx
@@ -904,7 +904,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="19" t="n">
-        <v>45406</v>
+        <v>45436</v>
       </c>
       <c r="F1" s="40" t="n"/>
       <c r="G1" s="40" t="n"/>
@@ -988,7 +988,7 @@
       </c>
       <c r="C33" s="44" t="n"/>
       <c r="D33" s="9" t="n">
-        <v>3287.585</v>
+        <v>5634.136</v>
       </c>
     </row>
     <row r="34" ht="16.5" customHeight="1" s="42">
@@ -1002,7 +1002,7 @@
       </c>
       <c r="C34" s="44" t="n"/>
       <c r="D34" s="9" t="n">
-        <v>2470.096</v>
+        <v>4233.155</v>
       </c>
     </row>
     <row r="35" ht="16.5" customHeight="1" s="42">
@@ -1016,7 +1016,7 @@
       </c>
       <c r="C35" s="44" t="n"/>
       <c r="D35" s="9" t="n">
-        <v>2131.561</v>
+        <v>3652.985</v>
       </c>
     </row>
     <row r="36" ht="16.5" customHeight="1" s="42">
@@ -1030,7 +1030,7 @@
       </c>
       <c r="C36" s="44" t="n"/>
       <c r="D36" s="9" t="n">
-        <v>1914.227</v>
+        <v>3280.528</v>
       </c>
     </row>
     <row r="37" ht="16.5" customHeight="1" s="42">
@@ -1044,7 +1044,7 @@
       </c>
       <c r="C37" s="44" t="n"/>
       <c r="D37" s="9" t="n">
-        <v>1914.227</v>
+        <v>3280.528</v>
       </c>
     </row>
     <row r="38" ht="16.5" customHeight="1" s="42">
@@ -1058,7 +1058,7 @@
       </c>
       <c r="C38" s="44" t="n"/>
       <c r="D38" s="9" t="n">
-        <v>1614.548</v>
+        <v>2766.95</v>
       </c>
     </row>
     <row r="39" ht="16.5" customHeight="1" s="42">
@@ -1072,7 +1072,7 @@
       </c>
       <c r="C39" s="44" t="n"/>
       <c r="D39" s="9" t="n">
-        <v>1614.548</v>
+        <v>2766.95</v>
       </c>
     </row>
     <row r="40" ht="16.5" customHeight="1" s="42">
@@ -1086,7 +1086,7 @@
       </c>
       <c r="C40" s="44" t="n"/>
       <c r="D40" s="9" t="n">
-        <v>1614.548</v>
+        <v>2766.95</v>
       </c>
     </row>
     <row r="41" ht="16.5" customHeight="1" s="42">
@@ -1100,7 +1100,7 @@
       </c>
       <c r="C41" s="44" t="n"/>
       <c r="D41" s="9" t="n">
-        <v>1614.548</v>
+        <v>2766.95</v>
       </c>
     </row>
     <row r="42" ht="16.5" customHeight="1" s="42">
@@ -1114,7 +1114,7 @@
       </c>
       <c r="C42" s="44" t="n"/>
       <c r="D42" s="9" t="n">
-        <v>1614.548</v>
+        <v>2766.95</v>
       </c>
     </row>
     <row r="43" ht="16.5" customHeight="1" s="42">
@@ -1128,7 +1128,7 @@
       </c>
       <c r="C43" s="44" t="n"/>
       <c r="D43" s="9" t="n">
-        <v>1614.548</v>
+        <v>2766.95</v>
       </c>
     </row>
     <row r="44" ht="16.5" customHeight="1" s="42">
@@ -1144,7 +1144,7 @@
       </c>
       <c r="C44" s="44" t="n"/>
       <c r="D44" s="9" t="n">
-        <v>1614.548</v>
+        <v>2766.95</v>
       </c>
     </row>
     <row r="45" ht="16.5" customHeight="1" s="42">
@@ -1160,7 +1160,7 @@
       </c>
       <c r="C45" s="44" t="n"/>
       <c r="D45" s="9" t="n">
-        <v>1926.763</v>
+        <v>3302.011</v>
       </c>
     </row>
     <row r="46" ht="16.5" customHeight="1" s="42">
@@ -1176,7 +1176,7 @@
       </c>
       <c r="C46" s="44" t="n"/>
       <c r="D46" s="9" t="n">
-        <v>1926.763</v>
+        <v>3302.011</v>
       </c>
     </row>
     <row r="47" ht="16.5" customHeight="1" s="42">
@@ -1192,7 +1192,7 @@
       </c>
       <c r="C47" s="44" t="n"/>
       <c r="D47" s="9" t="n">
-        <v>1926.763</v>
+        <v>3302.011</v>
       </c>
     </row>
     <row r="49" ht="18" customHeight="1" s="42">
@@ -1234,7 +1234,7 @@
       </c>
       <c r="C51" s="44" t="n"/>
       <c r="D51" s="9" t="n">
-        <v>2808.644</v>
+        <v>4813.344</v>
       </c>
     </row>
     <row r="52" ht="18" customHeight="1" s="42">
@@ -1248,7 +1248,7 @@
       </c>
       <c r="C52" s="44" t="n"/>
       <c r="D52" s="9" t="n">
-        <v>2553.696</v>
+        <v>4376.426</v>
       </c>
     </row>
     <row r="53" ht="23.25" customHeight="1" s="42">
@@ -1262,7 +1262,7 @@
       </c>
       <c r="C53" s="44" t="n"/>
       <c r="D53" s="9" t="n">
-        <v>2131.561</v>
+        <v>3652.985</v>
       </c>
       <c r="E53" s="10" t="n"/>
       <c r="F53" s="10" t="n"/>
@@ -1280,7 +1280,7 @@
       </c>
       <c r="C54" s="44" t="n"/>
       <c r="D54" s="9" t="n">
-        <v>2131.561</v>
+        <v>3652.985</v>
       </c>
       <c r="E54" s="11" t="n"/>
       <c r="F54" s="11" t="n"/>
@@ -1350,37 +1350,37 @@
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="B47:C47"/>
     <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D73:E73"/>
     <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B52:C52"/>
     <mergeCell ref="D77:E77"/>
+    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="A49:D49"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="D75:E75"/>
     <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="D76:E76"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="A31:D31"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B38:C38"/>
     <mergeCell ref="B34:C34"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="A49:D49"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D74:E74"/>
-    <mergeCell ref="B38:C38"/>
     <mergeCell ref="B37:C37"/>
     <mergeCell ref="B40:C40"/>
+    <mergeCell ref="D74:E74"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="D73:E73"/>
+    <mergeCell ref="B45:C45"/>
     <mergeCell ref="A10:H10"/>
     <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B35:C35"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
   <pageSetup orientation="portrait" paperSize="9" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>